<commit_message>
Presentation edit and user edit work now yay
</commit_message>
<xml_diff>
--- a/app-server/src/main/resources/presentations_responses.xlsx
+++ b/app-server/src/main/resources/presentations_responses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bushong/code/acmsac/app-server/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{11A18ED6-75B9-1748-A664-2AE2F04DCE84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FADAC57-4FA2-0341-B363-493AC2800931}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACM SAC 2020 presentation submi" sheetId="1" r:id="rId1"/>
@@ -14070,7 +14070,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -14909,14 +14909,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X372"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A295" workbookViewId="0">
-      <selection activeCell="P315" sqref="P315"/>
+    <sheetView tabSelected="1" topLeftCell="A369" workbookViewId="0">
+      <selection activeCell="G372" sqref="G372"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="27.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -15125,7 +15129,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -15190,7 +15194,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -15255,7 +15259,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" ht="404" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>89</v>
       </c>
@@ -15391,7 +15395,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>122</v>
       </c>
@@ -15518,7 +15522,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>153</v>
       </c>
@@ -15654,7 +15658,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>187</v>
       </c>
@@ -15710,7 +15714,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>201</v>
       </c>
@@ -15958,7 +15962,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>263</v>
       </c>
@@ -16017,7 +16021,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>277</v>
       </c>
@@ -16070,7 +16074,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:24" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>288</v>
       </c>
@@ -16138,7 +16142,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>305</v>
       </c>
@@ -16203,7 +16207,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>321</v>
       </c>
@@ -16271,7 +16275,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>338</v>
       </c>
@@ -16339,7 +16343,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>352</v>
       </c>
@@ -16404,7 +16408,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>366</v>
       </c>
@@ -16534,7 +16538,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>400</v>
       </c>
@@ -16608,7 +16612,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>419</v>
       </c>
@@ -16661,7 +16665,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>430</v>
       </c>
@@ -16732,7 +16736,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:24" ht="153" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>447</v>
       </c>
@@ -16803,7 +16807,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>466</v>
       </c>
@@ -16927,7 +16931,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>483</v>
       </c>
@@ -17375,7 +17379,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:24" ht="340" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>583</v>
       </c>
@@ -17499,7 +17503,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>602</v>
       </c>
@@ -17670,7 +17674,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>641</v>
       </c>
@@ -17856,7 +17860,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:24" ht="204" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>680</v>
       </c>
@@ -17927,7 +17931,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:24" ht="340" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>695</v>
       </c>
@@ -17983,7 +17987,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>705</v>
       </c>
@@ -18308,7 +18312,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>760</v>
       </c>
@@ -18382,7 +18386,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>777</v>
       </c>
@@ -18456,7 +18460,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>786</v>
       </c>
@@ -18530,7 +18534,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>787</v>
       </c>
@@ -18604,7 +18608,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:24" ht="187" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>788</v>
       </c>
@@ -18858,7 +18862,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>842</v>
       </c>
@@ -19100,7 +19104,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:24" ht="255" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>886</v>
       </c>
@@ -19460,7 +19464,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>954</v>
       </c>
@@ -19525,7 +19529,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>971</v>
       </c>
@@ -19584,7 +19588,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:24" ht="272" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>983</v>
       </c>
@@ -19652,7 +19656,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:24" ht="289" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>997</v>
       </c>
@@ -19723,7 +19727,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>1013</v>
       </c>
@@ -19785,7 +19789,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>1028</v>
       </c>
@@ -19915,7 +19919,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>1058</v>
       </c>
@@ -19989,7 +19993,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>1076</v>
       </c>
@@ -20045,7 +20049,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:24" ht="356" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>1089</v>
       </c>
@@ -20119,7 +20123,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="83" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:24" ht="272" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>1102</v>
       </c>
@@ -20190,7 +20194,7 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>1118</v>
       </c>
@@ -20264,7 +20268,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>1134</v>
       </c>
@@ -20335,7 +20339,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:24" ht="289" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>1149</v>
       </c>
@@ -20397,7 +20401,7 @@
         <v>201594643</v>
       </c>
     </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>1160</v>
       </c>
@@ -20630,7 +20634,7 @@
         <v>1211</v>
       </c>
     </row>
-    <row r="91" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>1212</v>
       </c>
@@ -20689,7 +20693,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="92" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>1223</v>
       </c>
@@ -20878,7 +20882,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="95" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>1261</v>
       </c>
@@ -20946,7 +20950,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="96" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>1275</v>
       </c>
@@ -20999,7 +21003,7 @@
         <v>1283</v>
       </c>
     </row>
-    <row r="97" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>1284</v>
       </c>
@@ -21058,7 +21062,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="98" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>1298</v>
       </c>
@@ -21176,7 +21180,7 @@
         <v>1321</v>
       </c>
     </row>
-    <row r="100" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:24" ht="404" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>1322</v>
       </c>
@@ -21300,7 +21304,7 @@
         <v>1345</v>
       </c>
     </row>
-    <row r="102" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:24" ht="404" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>1346</v>
       </c>
@@ -21362,7 +21366,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="103" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:24" ht="404" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>1347</v>
       </c>
@@ -21424,7 +21428,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="104" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:24" ht="340" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>1348</v>
       </c>
@@ -21486,7 +21490,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="105" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>1360</v>
       </c>
@@ -21551,7 +21555,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="106" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>1374</v>
       </c>
@@ -21675,7 +21679,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="108" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:24" ht="404" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>1400</v>
       </c>
@@ -21796,7 +21800,7 @@
         <v>1414</v>
       </c>
     </row>
-    <row r="110" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>1415</v>
       </c>
@@ -21923,7 +21927,7 @@
         <v>1441</v>
       </c>
     </row>
-    <row r="112" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>1442</v>
       </c>
@@ -21994,7 +21998,7 @@
         <v>1457</v>
       </c>
     </row>
-    <row r="113" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>1458</v>
       </c>
@@ -22115,7 +22119,7 @@
         <v>1474</v>
       </c>
     </row>
-    <row r="115" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>1475</v>
       </c>
@@ -22189,7 +22193,7 @@
         <v>1493</v>
       </c>
     </row>
-    <row r="116" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>1494</v>
       </c>
@@ -22245,7 +22249,7 @@
         <v>1505</v>
       </c>
     </row>
-    <row r="117" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:24" ht="170" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>1506</v>
       </c>
@@ -22378,7 +22382,7 @@
         <v>1530</v>
       </c>
     </row>
-    <row r="119" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>1531</v>
       </c>
@@ -22694,7 +22698,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="124" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>1594</v>
       </c>
@@ -22753,7 +22757,7 @@
         <v>1607</v>
       </c>
     </row>
-    <row r="125" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>1608</v>
       </c>
@@ -22880,7 +22884,7 @@
         <v>1633</v>
       </c>
     </row>
-    <row r="127" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:24" ht="272" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>1634</v>
       </c>
@@ -22939,7 +22943,7 @@
         <v>1647</v>
       </c>
     </row>
-    <row r="128" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>1648</v>
       </c>
@@ -23066,7 +23070,7 @@
         <v>1673</v>
       </c>
     </row>
-    <row r="130" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>1674</v>
       </c>
@@ -23125,7 +23129,7 @@
         <v>1685</v>
       </c>
     </row>
-    <row r="131" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:24" ht="356" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>1686</v>
       </c>
@@ -23267,7 +23271,7 @@
         <v>1714</v>
       </c>
     </row>
-    <row r="133" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>1715</v>
       </c>
@@ -23379,7 +23383,7 @@
         <v>1736</v>
       </c>
     </row>
-    <row r="135" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>1737</v>
       </c>
@@ -23618,7 +23622,7 @@
         <v>1784</v>
       </c>
     </row>
-    <row r="139" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>1785</v>
       </c>
@@ -23795,7 +23799,7 @@
         <v>1824</v>
       </c>
     </row>
-    <row r="142" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>1825</v>
       </c>
@@ -24037,7 +24041,7 @@
         <v>1870</v>
       </c>
     </row>
-    <row r="146" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:24" ht="404" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>1871</v>
       </c>
@@ -24170,7 +24174,7 @@
         <v>1889</v>
       </c>
     </row>
-    <row r="148" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:24" ht="187" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>1890</v>
       </c>
@@ -24294,7 +24298,7 @@
         <v>1913</v>
       </c>
     </row>
-    <row r="150" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>1914</v>
       </c>
@@ -24353,7 +24357,7 @@
         <v>1925</v>
       </c>
     </row>
-    <row r="151" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>1926</v>
       </c>
@@ -24480,7 +24484,7 @@
         <v>1952</v>
       </c>
     </row>
-    <row r="153" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:24" ht="388" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>1953</v>
       </c>
@@ -24604,7 +24608,7 @@
         <v>1975</v>
       </c>
     </row>
-    <row r="155" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>1976</v>
       </c>
@@ -24722,7 +24726,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="157" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>1999</v>
       </c>
@@ -24778,7 +24782,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="158" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>2011</v>
       </c>
@@ -24831,7 +24835,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="159" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:24" ht="255" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>2020</v>
       </c>
@@ -24973,7 +24977,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="161" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>2051</v>
       </c>
@@ -25041,7 +25045,7 @@
         <v>2062</v>
       </c>
     </row>
-    <row r="162" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:24" ht="221" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>2063</v>
       </c>
@@ -25153,7 +25157,7 @@
         <v>2085</v>
       </c>
     </row>
-    <row r="164" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>2086</v>
       </c>
@@ -25401,7 +25405,7 @@
         <v>2137</v>
       </c>
     </row>
-    <row r="168" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>2138</v>
       </c>
@@ -25935,7 +25939,7 @@
         <v>2242</v>
       </c>
     </row>
-    <row r="177" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>2243</v>
       </c>
@@ -26003,7 +26007,7 @@
         <v>2256</v>
       </c>
     </row>
-    <row r="178" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>2257</v>
       </c>
@@ -26195,7 +26199,7 @@
         <v>2294</v>
       </c>
     </row>
-    <row r="181" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>2295</v>
       </c>
@@ -26260,7 +26264,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="182" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>2311</v>
       </c>
@@ -26387,7 +26391,7 @@
         <v>2193</v>
       </c>
     </row>
-    <row r="184" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>2334</v>
       </c>
@@ -26697,7 +26701,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="189" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>2383</v>
       </c>
@@ -26836,7 +26840,7 @@
         <v>2413</v>
       </c>
     </row>
-    <row r="191" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:24" ht="221" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>2414</v>
       </c>
@@ -27143,7 +27147,7 @@
         <v>2458</v>
       </c>
     </row>
-    <row r="196" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>2459</v>
       </c>
@@ -27674,7 +27678,7 @@
         <v>2516</v>
       </c>
     </row>
-    <row r="205" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>2517</v>
       </c>
@@ -27795,7 +27799,7 @@
         <v>2539</v>
       </c>
     </row>
-    <row r="207" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:24" ht="272" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>2541</v>
       </c>
@@ -27854,7 +27858,7 @@
         <v>2550</v>
       </c>
     </row>
-    <row r="208" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:24" ht="136" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>2551</v>
       </c>
@@ -27922,7 +27926,7 @@
         <v>2553</v>
       </c>
     </row>
-    <row r="209" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>2554</v>
       </c>
@@ -27984,7 +27988,7 @@
         <v>2567</v>
       </c>
     </row>
-    <row r="210" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>2568</v>
       </c>
@@ -28492,7 +28496,7 @@
         <v>2374</v>
       </c>
     </row>
-    <row r="218" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>2639</v>
       </c>
@@ -28551,7 +28555,7 @@
         <v>2651</v>
       </c>
     </row>
-    <row r="219" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>2652</v>
       </c>
@@ -28731,7 +28735,7 @@
         <v>2681</v>
       </c>
     </row>
-    <row r="222" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>2682</v>
       </c>
@@ -28796,7 +28800,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="223" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:24" ht="323" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>2685</v>
       </c>
@@ -28855,7 +28859,7 @@
         <v>2695</v>
       </c>
     </row>
-    <row r="224" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>2696</v>
       </c>
@@ -28914,7 +28918,7 @@
         <v>2706</v>
       </c>
     </row>
-    <row r="225" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:24" ht="323" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>2707</v>
       </c>
@@ -29150,7 +29154,7 @@
         <v>2728</v>
       </c>
     </row>
-    <row r="229" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>2729</v>
       </c>
@@ -29203,7 +29207,7 @@
         <v>2739</v>
       </c>
     </row>
-    <row r="230" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>2740</v>
       </c>
@@ -29672,7 +29676,7 @@
         <v>2788</v>
       </c>
     </row>
-    <row r="238" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>2789</v>
       </c>
@@ -29734,7 +29738,7 @@
         <v>2796</v>
       </c>
     </row>
-    <row r="239" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>2797</v>
       </c>
@@ -29796,7 +29800,7 @@
         <v>2808</v>
       </c>
     </row>
-    <row r="240" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>2809</v>
       </c>
@@ -29920,7 +29924,7 @@
         <v>2834</v>
       </c>
     </row>
-    <row r="242" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:24" ht="272" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>2835</v>
       </c>
@@ -30029,7 +30033,7 @@
         <v>2852</v>
       </c>
     </row>
-    <row r="244" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>2853</v>
       </c>
@@ -30088,7 +30092,7 @@
         <v>2528</v>
       </c>
     </row>
-    <row r="245" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:24" ht="272" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>2854</v>
       </c>
@@ -30159,7 +30163,7 @@
         <v>2858</v>
       </c>
     </row>
-    <row r="246" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>2859</v>
       </c>
@@ -30327,7 +30331,7 @@
         <v>2891</v>
       </c>
     </row>
-    <row r="249" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:24" ht="238" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>2892</v>
       </c>
@@ -30439,7 +30443,7 @@
         <v>2908</v>
       </c>
     </row>
-    <row r="251" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>2909</v>
       </c>
@@ -30696,7 +30700,7 @@
         <v>2954</v>
       </c>
     </row>
-    <row r="255" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>2955</v>
       </c>
@@ -30832,7 +30836,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="257" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>2965</v>
       </c>
@@ -30906,7 +30910,7 @@
         <v>2980</v>
       </c>
     </row>
-    <row r="258" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>2981</v>
       </c>
@@ -30977,7 +30981,7 @@
         <v>2996</v>
       </c>
     </row>
-    <row r="259" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>2997</v>
       </c>
@@ -31095,7 +31099,7 @@
         <v>3017</v>
       </c>
     </row>
-    <row r="261" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>3018</v>
       </c>
@@ -31160,7 +31164,7 @@
         <v>1660</v>
       </c>
     </row>
-    <row r="262" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>3022</v>
       </c>
@@ -31234,7 +31238,7 @@
         <v>3038</v>
       </c>
     </row>
-    <row r="263" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:24" ht="323" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>3039</v>
       </c>
@@ -31588,7 +31592,7 @@
         <v>3091</v>
       </c>
     </row>
-    <row r="269" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>3092</v>
       </c>
@@ -32028,7 +32032,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="276" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>3166</v>
       </c>
@@ -32081,7 +32085,7 @@
         <v>3175</v>
       </c>
     </row>
-    <row r="277" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>3176</v>
       </c>
@@ -32385,7 +32389,7 @@
         <v>3225</v>
       </c>
     </row>
-    <row r="282" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>3226</v>
       </c>
@@ -32506,7 +32510,7 @@
         <v>3214</v>
       </c>
     </row>
-    <row r="284" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:24" ht="340" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>3241</v>
       </c>
@@ -32624,7 +32628,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="286" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:24" ht="136" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>3255</v>
       </c>
@@ -32748,7 +32752,7 @@
         <v>3276</v>
       </c>
     </row>
-    <row r="288" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>3277</v>
       </c>
@@ -32804,7 +32808,7 @@
         <v>3283</v>
       </c>
     </row>
-    <row r="289" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>3284</v>
       </c>
@@ -32875,7 +32879,7 @@
         <v>3296</v>
       </c>
     </row>
-    <row r="290" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>3298</v>
       </c>
@@ -32934,7 +32938,7 @@
         <v>3308</v>
       </c>
     </row>
-    <row r="291" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>3309</v>
       </c>
@@ -33123,7 +33127,7 @@
         <v>3339</v>
       </c>
     </row>
-    <row r="294" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>3340</v>
       </c>
@@ -33253,7 +33257,7 @@
         <v>3364</v>
       </c>
     </row>
-    <row r="296" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>3365</v>
       </c>
@@ -33368,7 +33372,7 @@
         <v>3384</v>
       </c>
     </row>
-    <row r="298" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:24" ht="170" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>3385</v>
       </c>
@@ -33424,7 +33428,7 @@
         <v>3395</v>
       </c>
     </row>
-    <row r="299" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:24" ht="170" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>3396</v>
       </c>
@@ -33480,7 +33484,7 @@
         <v>3395</v>
       </c>
     </row>
-    <row r="300" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>3397</v>
       </c>
@@ -33539,7 +33543,7 @@
         <v>2528</v>
       </c>
     </row>
-    <row r="301" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>3398</v>
       </c>
@@ -33610,7 +33614,7 @@
         <v>3414</v>
       </c>
     </row>
-    <row r="302" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>3415</v>
       </c>
@@ -33817,7 +33821,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="305" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:24" ht="170" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>3438</v>
       </c>
@@ -33888,7 +33892,7 @@
         <v>3452</v>
       </c>
     </row>
-    <row r="306" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>3453</v>
       </c>
@@ -33947,7 +33951,7 @@
         <v>3463</v>
       </c>
     </row>
-    <row r="307" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:24" ht="289" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>3464</v>
       </c>
@@ -34003,7 +34007,7 @@
         <v>3472</v>
       </c>
     </row>
-    <row r="308" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:24" ht="372" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>3473</v>
       </c>
@@ -34168,7 +34172,7 @@
         <v>3504</v>
       </c>
     </row>
-    <row r="311" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>3505</v>
       </c>
@@ -34348,7 +34352,7 @@
         <v>3540</v>
       </c>
     </row>
-    <row r="314" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>3541</v>
       </c>
@@ -34516,7 +34520,7 @@
         <v>3567</v>
       </c>
     </row>
-    <row r="317" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>3568</v>
       </c>
@@ -34708,7 +34712,7 @@
         <v>3606</v>
       </c>
     </row>
-    <row r="320" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:24" ht="255" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>3607</v>
       </c>
@@ -34767,7 +34771,7 @@
         <v>3617</v>
       </c>
     </row>
-    <row r="321" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>3618</v>
       </c>
@@ -34841,7 +34845,7 @@
         <v>3634</v>
       </c>
     </row>
-    <row r="322" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>3635</v>
       </c>
@@ -34962,7 +34966,7 @@
         <v>2775</v>
       </c>
     </row>
-    <row r="324" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:24" ht="323" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>3648</v>
       </c>
@@ -35021,7 +35025,7 @@
         <v>3650</v>
       </c>
     </row>
-    <row r="325" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:24" ht="170" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>3651</v>
       </c>
@@ -35216,7 +35220,7 @@
         <v>2357</v>
       </c>
     </row>
-    <row r="328" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:24" ht="306" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>3665</v>
       </c>
@@ -35281,7 +35285,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="329" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>3679</v>
       </c>
@@ -35343,7 +35347,7 @@
         <v>3691</v>
       </c>
     </row>
-    <row r="330" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:24" ht="340" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>3692</v>
       </c>
@@ -35408,7 +35412,7 @@
         <v>3704</v>
       </c>
     </row>
-    <row r="331" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:24" ht="255" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>3705</v>
       </c>
@@ -35520,7 +35524,7 @@
         <v>3714</v>
       </c>
     </row>
-    <row r="333" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>3715</v>
       </c>
@@ -35783,7 +35787,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="337" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>3748</v>
       </c>
@@ -36111,7 +36115,7 @@
         <v>3809</v>
       </c>
     </row>
-    <row r="342" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>3810</v>
       </c>
@@ -36176,7 +36180,7 @@
         <v>3814</v>
       </c>
     </row>
-    <row r="343" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>3815</v>
       </c>
@@ -36244,7 +36248,7 @@
         <v>3827</v>
       </c>
     </row>
-    <row r="344" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>3828</v>
       </c>
@@ -36306,7 +36310,7 @@
         <v>3838</v>
       </c>
     </row>
-    <row r="345" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>3839</v>
       </c>
@@ -36374,7 +36378,7 @@
         <v>2256</v>
       </c>
     </row>
-    <row r="346" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>3842</v>
       </c>
@@ -36448,7 +36452,7 @@
         <v>3848</v>
       </c>
     </row>
-    <row r="347" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>3849</v>
       </c>
@@ -36510,7 +36514,7 @@
         <v>3860</v>
       </c>
     </row>
-    <row r="348" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>3861</v>
       </c>
@@ -36575,7 +36579,7 @@
         <v>3868</v>
       </c>
     </row>
-    <row r="349" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:24" ht="221" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>3869</v>
       </c>
@@ -36637,7 +36641,7 @@
         <v>3225</v>
       </c>
     </row>
-    <row r="350" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>3871</v>
       </c>
@@ -36699,7 +36703,7 @@
         <v>3882</v>
       </c>
     </row>
-    <row r="351" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:24" ht="306" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>3883</v>
       </c>
@@ -36761,7 +36765,7 @@
         <v>3677</v>
       </c>
     </row>
-    <row r="352" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:24" ht="306" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>3885</v>
       </c>
@@ -36823,7 +36827,7 @@
         <v>3677</v>
       </c>
     </row>
-    <row r="353" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:24" ht="404" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>3889</v>
       </c>
@@ -36888,7 +36892,7 @@
         <v>3902</v>
       </c>
     </row>
-    <row r="354" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
         <v>3903</v>
       </c>
@@ -36950,7 +36954,7 @@
         <v>3913</v>
       </c>
     </row>
-    <row r="355" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:24" ht="255" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
         <v>3914</v>
       </c>
@@ -37015,7 +37019,7 @@
         <v>3926</v>
       </c>
     </row>
-    <row r="356" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
         <v>3927</v>
       </c>
@@ -37083,7 +37087,7 @@
         <v>3940</v>
       </c>
     </row>
-    <row r="357" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:24" ht="102" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
         <v>3941</v>
       </c>
@@ -37157,7 +37161,7 @@
         <v>3956</v>
       </c>
     </row>
-    <row r="358" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
         <v>3957</v>
       </c>
@@ -37216,7 +37220,7 @@
         <v>3968</v>
       </c>
     </row>
-    <row r="359" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:24" ht="136" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>3969</v>
       </c>
@@ -37284,7 +37288,7 @@
         <v>3981</v>
       </c>
     </row>
-    <row r="360" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
         <v>3982</v>
       </c>
@@ -37337,7 +37341,7 @@
         <v>1796</v>
       </c>
     </row>
-    <row r="361" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
         <v>3989</v>
       </c>
@@ -37470,7 +37474,7 @@
         <v>4015</v>
       </c>
     </row>
-    <row r="363" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:24" ht="372" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
         <v>4016</v>
       </c>
@@ -37535,7 +37539,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="364" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:24" ht="153" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
         <v>4020</v>
       </c>
@@ -37606,7 +37610,7 @@
         <v>3265</v>
       </c>
     </row>
-    <row r="365" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:24" ht="323" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>4023</v>
       </c>
@@ -37677,7 +37681,7 @@
         <v>4037</v>
       </c>
     </row>
-    <row r="366" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
         <v>4038</v>
       </c>
@@ -37742,7 +37746,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="367" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
         <v>4041</v>
       </c>
@@ -37801,7 +37805,7 @@
         <v>4053</v>
       </c>
     </row>
-    <row r="368" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:24" ht="306" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
         <v>4054</v>
       </c>
@@ -37854,7 +37858,7 @@
         <v>4057</v>
       </c>
     </row>
-    <row r="369" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
         <v>4058</v>
       </c>
@@ -37969,7 +37973,7 @@
         <v>2610</v>
       </c>
     </row>
-    <row r="371" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:24" ht="102" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
         <v>4069</v>
       </c>
@@ -38025,7 +38029,7 @@
         <v>4072</v>
       </c>
     </row>
-    <row r="372" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:24" ht="272" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
         <v>4073</v>
       </c>

</xml_diff>